<commit_message>
2021-07-02 JCS : suppression lien evento
</commit_message>
<xml_diff>
--- a/FulOverdueAndLostLoanLetter/FulOverdueAndLostLoanLetter-param-french.xlsx
+++ b/FulOverdueAndLostLoanLetter/FulOverdueAndLostLoanLetter-param-french.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="103">
   <si>
     <t>Activé</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>additional_info_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En raison du contexte sanitaire, la prise de rendez-vous est obligatoire. Vous pouvez sélectionner un créneau en suivant ce lien : </t>
   </si>
   <si>
     <t>fee_amount</t>
@@ -662,7 +659,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1061,7 +1060,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1075,13 +1074,13 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>42</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1095,13 +1094,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
         <v>43</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>44</v>
-      </c>
-      <c r="D22" t="s">
-        <v>45</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1115,13 +1114,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
         <v>46</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>47</v>
-      </c>
-      <c r="D23" t="s">
-        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1135,13 +1134,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>51</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1155,13 +1154,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
         <v>52</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>53</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1175,13 +1174,13 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
         <v>53</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -1195,13 +1194,13 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
         <v>56</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>57</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1215,13 +1214,13 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>61</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1235,13 +1234,13 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
         <v>60</v>
-      </c>
-      <c r="D29" t="s">
-        <v>61</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1255,13 +1254,13 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
         <v>63</v>
       </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
       <c r="D30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1275,13 +1274,13 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
         <v>65</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>66</v>
-      </c>
-      <c r="D31" t="s">
-        <v>67</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1295,13 +1294,13 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
         <v>68</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>69</v>
-      </c>
-      <c r="D32" t="s">
-        <v>70</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1315,13 +1314,13 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
         <v>71</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>72</v>
-      </c>
-      <c r="D33" t="s">
-        <v>73</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1335,13 +1334,13 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" t="s">
         <v>72</v>
-      </c>
-      <c r="D34" t="s">
-        <v>73</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1355,13 +1354,13 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
         <v>72</v>
-      </c>
-      <c r="D35" t="s">
-        <v>73</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1375,13 +1374,13 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" t="s">
         <v>76</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" t="s">
-        <v>77</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1395,13 +1394,13 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" t="s">
         <v>72</v>
-      </c>
-      <c r="D37" t="s">
-        <v>73</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -1415,13 +1414,13 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" t="s">
         <v>72</v>
-      </c>
-      <c r="D38" t="s">
-        <v>73</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -1435,13 +1434,13 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
         <v>80</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>81</v>
-      </c>
-      <c r="D39" t="s">
-        <v>82</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1455,13 +1454,13 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" t="s">
         <v>81</v>
-      </c>
-      <c r="D40" t="s">
-        <v>82</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1475,13 +1474,13 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" t="s">
         <v>81</v>
-      </c>
-      <c r="D41" t="s">
-        <v>82</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1495,13 +1494,13 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
         <v>81</v>
-      </c>
-      <c r="D42" t="s">
-        <v>82</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1515,13 +1514,13 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" t="s">
         <v>81</v>
-      </c>
-      <c r="D43" t="s">
-        <v>82</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1535,13 +1534,13 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" t="s">
         <v>87</v>
-      </c>
-      <c r="C44" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" t="s">
-        <v>88</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1555,16 +1554,16 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" t="s">
         <v>89</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" t="s">
         <v>90</v>
-      </c>
-      <c r="D45" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" t="s">
-        <v>91</v>
       </c>
       <c r="F45" s="1">
         <v>43865</v>
@@ -1575,13 +1574,13 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
         <v>92</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>93</v>
-      </c>
-      <c r="D46" t="s">
-        <v>94</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -1595,13 +1594,13 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
         <v>95</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>96</v>
-      </c>
-      <c r="D47" t="s">
-        <v>97</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -1615,13 +1614,13 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" t="s">
         <v>96</v>
-      </c>
-      <c r="D48" t="s">
-        <v>97</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
@@ -1635,13 +1634,13 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" t="s">
         <v>96</v>
-      </c>
-      <c r="D49" t="s">
-        <v>97</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -1655,13 +1654,13 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C50" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" t="s">
         <v>96</v>
-      </c>
-      <c r="D50" t="s">
-        <v>97</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
@@ -1675,13 +1674,13 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" t="s">
         <v>96</v>
-      </c>
-      <c r="D51" t="s">
-        <v>97</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -1695,13 +1694,13 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" t="s">
         <v>102</v>
-      </c>
-      <c r="C52" t="s">
-        <v>96</v>
-      </c>
-      <c r="D52" t="s">
-        <v>103</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>

</xml_diff>